<commit_message>
Add Exp Paper screenshots
</commit_message>
<xml_diff>
--- a/Document/WordSentence Count for English and Filipino.xlsx
+++ b/Document/WordSentence Count for English and Filipino.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showObjects="none"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rihanna\Documents\Pol\ThesisIt\SumMe\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="5385" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SENTENCE COUNT(ENG)" sheetId="2" r:id="rId1"/>
@@ -14,9 +19,9 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="125">
   <si>
     <t>English1</t>
   </si>
@@ -399,19 +404,16 @@
   </si>
   <si>
     <t>Filipino40</t>
-  </si>
-  <si>
-    <t>1+D69</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,13 +506,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,74 +573,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -692,7 +626,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FBFBFB"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -939,21 +873,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -962,15 +896,15 @@
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -985,7 +919,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +934,7 @@
         <v>0.35294117647058826</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +949,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1030,7 +964,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +979,7 @@
         <v>0.38095238095238093</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1060,7 +994,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1009,7 @@
         <v>0.37931034482758619</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1024,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1039,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1120,13 +1054,13 @@
         <v>0.38461538461538464</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1075,7 @@
         <v>0.38709677419354838</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1090,7 @@
         <v>0.52173913043478259</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1171,7 +1105,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1120,7 @@
         <v>0.43396226415094341</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1135,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1150,7 @@
         <v>0.29411764705882354</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1231,7 +1165,7 @@
         <v>0.45714285714285713</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1180,7 @@
         <v>0.44827586206896552</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1261,7 +1195,7 @@
         <v>0.34883720930232559</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1276,7 +1210,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1291,7 +1225,7 @@
         <v>0.37931034482758619</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1306,7 +1240,7 @@
         <v>0.5757575757575758</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1321,7 +1255,7 @@
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1336,13 +1270,13 @@
         <v>0.51851851851851849</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1357,7 +1291,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1372,7 +1306,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1387,7 +1321,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1402,7 +1336,7 @@
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1417,7 +1351,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1432,7 +1366,7 @@
         <v>0.40476190476190477</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1447,7 +1381,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1462,7 +1396,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1477,7 +1411,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1492,7 +1426,7 @@
         <v>0.46153846153846156</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1507,7 +1441,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1522,7 +1456,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1537,7 +1471,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1552,7 +1486,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1567,7 +1501,7 @@
         <v>0.41379310344827586</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1582,7 +1516,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1531,7 @@
         <v>0.29411764705882354</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1612,7 +1546,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1627,7 +1561,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1642,7 +1576,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1657,7 +1591,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1672,7 +1606,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1687,7 +1621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1702,7 +1636,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1717,7 +1651,7 @@
         <v>0.10483870967741936</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1732,7 +1666,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1747,7 +1681,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1762,7 +1696,7 @@
         <v>0.34615384615384615</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1777,7 +1711,7 @@
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1792,7 +1726,7 @@
         <v>0.47368421052631576</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1807,7 +1741,7 @@
         <v>0.39285714285714285</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1822,7 +1756,7 @@
         <v>0.34146341463414637</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1837,7 +1771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1852,7 +1786,7 @@
         <v>0.53846153846153844</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1867,7 +1801,7 @@
         <v>0.44680851063829785</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1882,7 +1816,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1897,7 +1831,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1912,7 +1846,7 @@
         <v>0.52173913043478259</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1927,7 +1861,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1942,7 +1876,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1957,7 +1891,7 @@
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1972,7 +1906,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +1921,7 @@
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -2002,7 +1936,7 @@
         <v>0.20370370370370369</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -2024,14 +1958,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -2039,15 +1973,15 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2058,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2073,7 +2007,7 @@
         <v>0.14803625377643503</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2088,7 +2022,7 @@
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2103,7 +2037,7 @@
         <v>0.12621359223300971</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2118,7 +2052,7 @@
         <v>0.22535211267605634</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2133,7 +2067,7 @@
         <v>0.24130434782608695</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2148,7 +2082,7 @@
         <v>0.11050477489768076</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2097,7 @@
         <v>0.15549597855227881</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2178,7 +2112,7 @@
         <v>0.17948717948717949</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2193,13 +2127,13 @@
         <v>0.15510204081632653</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2148,7 @@
         <v>0.14010989010989011</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2229,7 +2163,7 @@
         <v>0.14780600461893764</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2244,7 +2178,7 @@
         <v>9.4117647058823528E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2193,7 @@
         <v>0.1645813282001925</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2274,7 +2208,7 @@
         <v>0.15953947368421054</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2289,7 +2223,7 @@
         <v>9.815950920245399E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2304,7 +2238,7 @@
         <v>0.15544041450777202</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2319,7 +2253,7 @@
         <v>0.15082956259426847</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2334,7 +2268,7 @@
         <v>0.17391304347826086</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2349,7 +2283,7 @@
         <v>0.15204678362573099</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2364,7 +2298,7 @@
         <v>0.16971713810316139</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2379,7 +2313,7 @@
         <v>0.19359145527369825</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2394,7 +2328,7 @@
         <v>0.1388888888888889</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2409,13 +2343,13 @@
         <v>0.12044374009508717</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2430,7 +2364,7 @@
         <v>0.13389121338912133</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2445,7 +2379,7 @@
         <v>0.15264797507788161</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2460,7 +2394,7 @@
         <v>0.18666666666666668</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2475,7 +2409,7 @@
         <v>0.12737642585551331</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2490,7 +2424,7 @@
         <v>0.13225058004640372</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2505,7 +2439,7 @@
         <v>0.17948717948717949</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +2454,7 @@
         <v>0.14772727272727273</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2535,7 +2469,7 @@
         <v>0.22038567493112948</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2550,7 +2484,7 @@
         <v>0.16339869281045752</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2565,7 +2499,7 @@
         <v>0.11728395061728394</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2580,7 +2514,7 @@
         <v>0.16267942583732056</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2595,7 +2529,7 @@
         <v>0.18590522478736329</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2610,7 +2544,7 @@
         <v>0.31958762886597936</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2625,7 +2559,7 @@
         <v>0.151618398637138</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2640,7 +2574,7 @@
         <v>0.1334355828220859</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2655,7 +2589,7 @@
         <v>8.8560885608856083E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2670,7 +2604,7 @@
         <v>0.11138014527845036</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2685,7 +2619,7 @@
         <v>0.15171503957783641</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2700,7 +2634,7 @@
         <v>0.15217391304347827</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2715,7 +2649,7 @@
         <v>0.16753022452504318</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2730,7 +2664,7 @@
         <v>0.11587982832618025</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2745,7 +2679,7 @@
         <v>0.13150684931506848</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2760,7 +2694,7 @@
         <v>0.17886178861788618</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2775,7 +2709,7 @@
         <v>0.14642082429501085</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2790,7 +2724,7 @@
         <v>0.13493253373313344</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2805,7 +2739,7 @@
         <v>0.14355231143552311</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2820,7 +2754,7 @@
         <v>0.15880893300248139</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2835,7 +2769,7 @@
         <v>0.15324675324675324</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2850,7 +2784,7 @@
         <v>0.15966386554621848</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2865,7 +2799,7 @@
         <v>0.18010752688172044</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2880,7 +2814,7 @@
         <v>0.17077798861480076</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2895,7 +2829,7 @@
         <v>0.14350453172205438</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -2910,7 +2844,7 @@
         <v>7.8260869565217397E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2925,7 +2859,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2940,7 +2874,7 @@
         <v>0.17550058892815076</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2955,7 +2889,7 @@
         <v>6.8965517241379309E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2970,7 +2904,7 @@
         <v>0.15601023017902813</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2985,7 +2919,7 @@
         <v>0.1524822695035461</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -3000,7 +2934,7 @@
         <v>0.17411764705882352</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -3015,7 +2949,7 @@
         <v>0.18596491228070175</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -3030,7 +2964,7 @@
         <v>0.24242424242424243</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -3045,7 +2979,7 @@
         <v>0.13490364025695931</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -3060,7 +2994,7 @@
         <v>0.1415929203539823</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -3075,7 +3009,7 @@
         <v>0.11424731182795698</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3097,14 +3031,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -3112,15 +3046,15 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3131,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3146,7 +3080,7 @@
         <v>0.29559748427672955</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -3161,7 +3095,7 @@
         <v>9.0425531914893623E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -3176,7 +3110,7 @@
         <v>3.6809815950920248E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -3191,7 +3125,7 @@
         <v>5.208333333333333E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -3206,7 +3140,7 @@
         <v>1.282051282051282E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -3221,7 +3155,7 @@
         <v>6.3176895306859202E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -3236,7 +3170,7 @@
         <v>4.9689440993788817E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -3251,7 +3185,7 @@
         <v>0.15471698113207547</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -3266,13 +3200,13 @@
         <v>4.7808764940239043E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -3287,7 +3221,7 @@
         <v>4.4334975369458129E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -3302,7 +3236,7 @@
         <v>0.12337662337662338</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -3317,7 +3251,7 @@
         <v>7.0512820512820512E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -3332,7 +3266,7 @@
         <v>5.0314465408805034E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -3347,7 +3281,7 @@
         <v>0.14795918367346939</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -3362,7 +3296,7 @@
         <v>0.29559748427672955</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -3377,7 +3311,7 @@
         <v>0.10638297872340426</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -3392,7 +3326,7 @@
         <v>3.6809815950920248E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -3407,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -3422,7 +3356,7 @@
         <v>5.3191489361702128E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -3437,7 +3371,7 @@
         <v>9.4240837696335081E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -3452,7 +3386,7 @@
         <v>0.19108280254777071</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -3467,7 +3401,7 @@
         <v>4.9689440993788817E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -3482,7 +3416,7 @@
         <v>0.11976047904191617</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -3497,7 +3431,7 @@
         <v>4.6296296296296294E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -3512,7 +3446,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -3527,7 +3461,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -3542,7 +3476,7 @@
         <v>4.5714285714285714E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -3557,7 +3491,7 @@
         <v>7.7519379844961239E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -3572,7 +3506,7 @@
         <v>0.1623931623931624</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -3587,7 +3521,7 @@
         <v>4.9645390070921988E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -3602,7 +3536,7 @@
         <v>0.1834862385321101</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -3617,7 +3551,7 @@
         <v>4.5751633986928102E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -3632,7 +3566,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -3647,7 +3581,7 @@
         <v>0.12111801242236025</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -3662,7 +3596,7 @@
         <v>8.2278481012658222E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -3677,7 +3611,7 @@
         <v>1.7167381974248927E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -3692,7 +3626,7 @@
         <v>0.11538461538461539</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -3707,7 +3641,7 @@
         <v>3.3707865168539325E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -3722,181 +3656,181 @@
         <v>2.5787965616045846E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2" t="e">
         <f t="shared" ref="D68:D72" si="1">C68/B68</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="4:4">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="4:4">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="4:4">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="4:4">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3912,14 +3846,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -3927,15 +3861,15 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3946,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3961,7 +3895,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -3976,7 +3910,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -3991,7 +3925,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -4006,7 +3940,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -4021,7 +3955,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -4036,7 +3970,7 @@
         <v>0.34782608695652173</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -4051,7 +3985,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -4066,7 +4000,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -4081,13 +4015,13 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -4102,7 +4036,7 @@
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -4117,7 +4051,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -4132,7 +4066,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -4147,7 +4081,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -4162,7 +4096,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -4177,7 +4111,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>101</v>
       </c>
@@ -4192,7 +4126,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>102</v>
       </c>
@@ -4207,7 +4141,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -4222,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -4237,7 +4171,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -4252,7 +4186,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -4267,7 +4201,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -4282,7 +4216,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -4297,7 +4231,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -4312,7 +4246,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -4327,7 +4261,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -4342,7 +4276,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4357,7 +4291,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4372,7 +4306,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4387,7 +4321,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4402,7 +4336,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -4417,7 +4351,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -4432,7 +4366,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -4447,7 +4381,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>119</v>
       </c>
@@ -4462,7 +4396,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>120</v>
       </c>
@@ -4477,7 +4411,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -4492,7 +4426,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -4507,7 +4441,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -4522,7 +4456,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -4537,94 +4471,94 @@
         <v>0.6428571428571429</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
   </sheetData>
@@ -4637,14 +4571,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I70"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
@@ -4657,12 +4591,12 @@
     <col min="9" max="9" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -4691,7 +4625,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4720,7 +4654,7 @@
         <v>0.24990000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4749,7 +4683,7 @@
         <v>0.1666</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4778,7 +4712,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4807,7 +4741,7 @@
         <v>0.37490000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4817,8 +4751,8 @@
       <c r="C7" s="2">
         <v>0.37930000000000003</v>
       </c>
-      <c r="D7" t="s">
-        <v>125</v>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" s="4">
         <v>0.04</v>
@@ -4836,7 +4770,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4865,7 +4799,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4894,7 +4828,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4923,7 +4857,7 @@
         <v>0.24990000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4952,7 +4886,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4981,7 +4915,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -5010,7 +4944,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -5039,7 +4973,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -5068,7 +5002,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -5097,7 +5031,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -5126,7 +5060,7 @@
         <v>0.20830000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -5155,7 +5089,7 @@
         <v>0.32140000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -5184,7 +5118,7 @@
         <v>0.28560000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -5213,7 +5147,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -5242,7 +5176,7 @@
         <v>0.35709999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5271,7 +5205,7 @@
         <v>0.58330000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -5300,7 +5234,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -5329,7 +5263,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -5358,7 +5292,7 @@
         <v>0.2142</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -5387,7 +5321,7 @@
         <v>0.49990000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -5416,7 +5350,7 @@
         <v>0.49990000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -5445,7 +5379,7 @@
         <v>0.14280000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -5474,7 +5408,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -5503,7 +5437,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -5532,7 +5466,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -5561,7 +5495,7 @@
         <v>0.38879999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -5590,7 +5524,7 @@
         <v>0.20830000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -5619,7 +5553,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -5648,7 +5582,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -5677,7 +5611,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -5706,7 +5640,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -5735,7 +5669,7 @@
         <v>0.1666</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -5764,7 +5698,7 @@
         <v>0.37490000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -5793,7 +5727,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -5822,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -5851,7 +5785,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -5880,7 +5814,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -5909,7 +5843,7 @@
         <v>0.24990000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -5938,7 +5872,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -5967,7 +5901,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -5996,7 +5930,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -6025,7 +5959,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -6054,7 +5988,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -6083,7 +6017,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -6112,7 +6046,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -6141,7 +6075,7 @@
         <v>0.29160000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -6170,7 +6104,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -6199,7 +6133,7 @@
         <v>0.2399</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -6228,7 +6162,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -6257,7 +6191,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -6286,7 +6220,7 @@
         <v>7.1400000000000005E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -6315,7 +6249,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -6344,7 +6278,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -6373,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -6402,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -6431,7 +6365,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -6460,7 +6394,7 @@
         <v>0.56259999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -6489,7 +6423,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -6518,7 +6452,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -6547,7 +6481,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -6576,7 +6510,7 @@
         <v>8.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -6605,7 +6539,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>83</v>
       </c>
@@ -6619,7 +6553,7 @@
       </c>
       <c r="D70">
         <f>SUM(D3:D68)/68</f>
-        <v>0.45889264705882366</v>
+        <v>0.47359852941176483</v>
       </c>
       <c r="E70" s="4">
         <f>SUM(E3:E69)/68</f>
@@ -6652,14 +6586,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
@@ -6667,7 +6601,7 @@
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -6690,7 +6624,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -6713,30 +6647,30 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>0.22220000000000001</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0.25</v>
       </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -6759,7 +6693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -6782,7 +6716,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -6805,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -6828,7 +6762,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -6851,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -6874,7 +6808,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -6897,7 +6831,7 @@
         <v>0.41660000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -6920,7 +6854,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -6943,7 +6877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -6966,7 +6900,7 @@
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -6989,7 +6923,7 @@
         <v>0.1666</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -7012,7 +6946,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -7035,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -7058,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -7081,7 +7015,7 @@
         <v>0.1666</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -7104,7 +7038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -7127,7 +7061,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -7150,7 +7084,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -7173,7 +7107,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -7196,7 +7130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -7219,32 +7153,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
       <c r="B27">
-        <f>SUM(B3:B26)/30</f>
+        <f t="shared" ref="B27:G27" si="0">SUM(B3:B26)/30</f>
         <v>8.1306666666666666E-2</v>
       </c>
       <c r="C27">
-        <f>SUM(C3:C26)/30</f>
+        <f t="shared" si="0"/>
         <v>0.24673</v>
       </c>
       <c r="D27">
-        <f>SUM(D3:D26)/30</f>
+        <f t="shared" si="0"/>
         <v>0.19419666666666668</v>
       </c>
       <c r="E27">
-        <f>SUM(E3:E26)/30</f>
+        <f t="shared" si="0"/>
         <v>0.13444</v>
       </c>
       <c r="F27">
-        <f>SUM(F3:F26)/30</f>
+        <f t="shared" si="0"/>
         <v>8.1663333333333338E-2</v>
       </c>
       <c r="G27">
-        <f>SUM(G3:G26)/30</f>
+        <f t="shared" si="0"/>
         <v>0.10804666666666665</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated chapters 3 and 4
</commit_message>
<xml_diff>
--- a/Document/WordSentence Count for English and Filipino.xlsx
+++ b/Document/WordSentence Count for English and Filipino.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="126">
   <si>
     <t>English1</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>Filipino40</t>
+  </si>
+  <si>
+    <t>1+D69</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +455,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -485,27 +494,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -528,13 +545,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -659,8 +669,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G34" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="A2:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:G27" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A2:G27"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Filename"/>
     <tableColumn id="2" name="CW"/>
@@ -929,7 +939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -953,12 +963,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" s="1" t="s">
@@ -2030,12 +2040,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -3103,12 +3113,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -3918,12 +3928,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -3962,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D67" si="0">C4/B4</f>
+        <f t="shared" ref="D4:D42" si="0">C4/B4</f>
         <v>0.22222222222222221</v>
       </c>
     </row>
@@ -4631,7 +4641,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="I3" sqref="I3:I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4807,8 +4817,8 @@
       <c r="C7" s="2">
         <v>0.37930000000000003</v>
       </c>
-      <c r="D7">
-        <v>1.24</v>
+      <c r="D7" t="s">
+        <v>125</v>
       </c>
       <c r="E7" s="4">
         <v>0.04</v>
@@ -6609,7 +6619,7 @@
       </c>
       <c r="D70">
         <f>SUM(D3:D68)/68</f>
-        <v>0.47712794117647078</v>
+        <v>0.45889264705882366</v>
       </c>
       <c r="E70" s="4">
         <f>SUM(E3:E69)/68</f>
@@ -6643,10 +6653,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G34"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6658,25 +6668,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>82</v>
       </c>
     </row>
@@ -6704,40 +6714,40 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="11">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>0.22220000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>0.25</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5">
-        <v>3.6799999999999999E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="C5">
-        <v>7.6899999999999996E-2</v>
+        <v>0.1429</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -6751,39 +6761,39 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B6">
-        <v>5.1999999999999998E-3</v>
+        <v>6.3200000000000006E-2</v>
       </c>
       <c r="C6">
-        <v>0.1429</v>
+        <v>0.3478</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.14280000000000001</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B7">
-        <v>1.2800000000000001E-2</v>
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>0.1429</v>
+        <v>0.125</v>
       </c>
       <c r="D7">
-        <v>0.33329999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -6797,39 +6807,39 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B8">
-        <v>6.3200000000000006E-2</v>
+        <v>0.1547</v>
       </c>
       <c r="C8">
-        <v>0.3478</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="D8">
-        <v>0.14280000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B9">
-        <v>4.9700000000000001E-2</v>
+        <v>4.7800000000000002E-2</v>
       </c>
       <c r="C9">
-        <v>0.125</v>
+        <v>0.2727</v>
       </c>
       <c r="D9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6843,128 +6853,128 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B10">
-        <v>0.1547</v>
+        <v>4.4299999999999999E-2</v>
       </c>
       <c r="C10">
-        <v>0.45450000000000002</v>
+        <v>0.1429</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E10">
         <v>0.25</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G10">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B11">
-        <v>4.7800000000000002E-2</v>
+        <v>0.1234</v>
       </c>
       <c r="C11">
-        <v>0.2727</v>
+        <v>9.0899999999999995E-2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.41660000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B12">
-        <v>4.4299999999999999E-2</v>
+        <v>5.0299999999999997E-2</v>
       </c>
       <c r="C12">
-        <v>0.1429</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="D12">
         <v>0.33329999999999999</v>
       </c>
       <c r="E12">
-        <v>0.25</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="F12">
-        <v>0.25</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="G12">
-        <v>0.25</v>
+        <v>0.33329999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B13">
-        <v>0.1234</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="C13">
-        <v>9.0899999999999995E-2</v>
+        <v>0.375</v>
       </c>
       <c r="D13">
         <v>0.25</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0.41660000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B14">
-        <v>7.0499999999999993E-2</v>
+        <v>0.29559999999999997</v>
       </c>
       <c r="C14">
-        <v>0.16669999999999999</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B15">
-        <v>5.0299999999999997E-2</v>
+        <v>0.19109999999999999</v>
       </c>
       <c r="C15">
-        <v>0.16669999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="D15">
         <v>0.33329999999999999</v>
@@ -6973,67 +6983,67 @@
         <v>0.33329999999999999</v>
       </c>
       <c r="F15">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.33329999999999999</v>
+        <v>0.1666</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B16">
-        <v>0.14799999999999999</v>
+        <v>0.1198</v>
       </c>
       <c r="C16">
-        <v>0.375</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="D16">
-        <v>0.25</v>
+        <v>0.66659999999999997</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B17">
-        <v>0.29559999999999997</v>
+        <v>7.6399999999999996E-2</v>
       </c>
       <c r="C17">
-        <v>0.36359999999999998</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="D17">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="E17">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -7050,131 +7060,131 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B19">
-        <v>5.3199999999999997E-2</v>
+        <v>4.5699999999999998E-2</v>
       </c>
       <c r="C19">
-        <v>0.16669999999999999</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>0.1666</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B20">
-        <v>0.19109999999999999</v>
+        <v>7.7999999999999996E-3</v>
       </c>
       <c r="C20">
-        <v>0.6</v>
+        <v>8.3299999999999999E-2</v>
       </c>
       <c r="D20">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.1666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B21">
-        <v>0.1198</v>
+        <v>0.16239999999999999</v>
       </c>
       <c r="C21">
-        <v>0.33329999999999999</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="D21">
-        <v>0.66659999999999997</v>
+        <v>0.2</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G21">
-        <v>0.5</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B22">
-        <v>4.6300000000000001E-2</v>
+        <v>4.9599999999999998E-2</v>
       </c>
       <c r="C22">
-        <v>0.28570000000000001</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B23">
-        <v>7.6399999999999996E-2</v>
+        <v>0.1835</v>
       </c>
       <c r="C23">
-        <v>0.16669999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>0.25</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B24">
-        <v>6.25E-2</v>
+        <v>4.3499999999999997E-2</v>
       </c>
       <c r="C24">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="D24">
         <v>0.25</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -7188,214 +7198,53 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B25">
-        <v>4.5699999999999998E-2</v>
+        <v>0.1211</v>
       </c>
       <c r="C25">
-        <v>0.91669999999999996</v>
+        <v>0.42859999999999998</v>
       </c>
       <c r="D25">
         <v>0.2</v>
       </c>
       <c r="E25">
-        <v>0.33329999999999999</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.1666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="C26">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="B27">
-        <v>0.16239999999999999</v>
+        <f>SUM(B3:B26)/30</f>
+        <v>8.1306666666666666E-2</v>
       </c>
       <c r="C27">
-        <v>0.36359999999999998</v>
+        <f>SUM(C3:C26)/30</f>
+        <v>0.24673</v>
       </c>
       <c r="D27">
-        <v>0.2</v>
+        <f>SUM(D3:D26)/30</f>
+        <v>0.19419666666666668</v>
       </c>
       <c r="E27">
-        <v>0.375</v>
+        <f>SUM(E3:E26)/30</f>
+        <v>0.13444</v>
       </c>
       <c r="F27">
-        <v>0.25</v>
+        <f>SUM(F3:F26)/30</f>
+        <v>8.1663333333333338E-2</v>
       </c>
       <c r="G27">
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28">
-        <v>4.9599999999999998E-2</v>
-      </c>
-      <c r="C28">
-        <v>0.22220000000000001</v>
-      </c>
-      <c r="D28">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="E28">
-        <v>0.25</v>
-      </c>
-      <c r="F28">
-        <v>0.25</v>
-      </c>
-      <c r="G28">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29">
-        <v>0.1835</v>
-      </c>
-      <c r="C29">
-        <v>0.6</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0.25</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B30">
-        <v>4.58E-2</v>
-      </c>
-      <c r="C30">
-        <v>9.0899999999999995E-2</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31">
-        <v>4.3499999999999997E-2</v>
-      </c>
-      <c r="C31">
-        <v>0.33329999999999999</v>
-      </c>
-      <c r="D31">
-        <v>0.25</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32">
-        <v>0.1211</v>
-      </c>
-      <c r="C32">
-        <v>0.42859999999999998</v>
-      </c>
-      <c r="D32">
-        <v>0.2</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34">
-        <f>SUM(B3:B33)/30</f>
-        <v>8.9899999999999966E-2</v>
-      </c>
-      <c r="C34">
-        <f>SUM(C3:C33)/30</f>
-        <v>0.27772333333333332</v>
-      </c>
-      <c r="D34">
-        <f>SUM(D3:D33)/30</f>
-        <v>0.19419666666666668</v>
-      </c>
-      <c r="E34">
-        <f>SUM(E3:E33)/30</f>
-        <v>0.13444</v>
-      </c>
-      <c r="F34">
-        <f>SUM(F3:F33)/30</f>
-        <v>8.1663333333333338E-2</v>
-      </c>
-      <c r="G34">
-        <f>SUM(G3:G33)/30</f>
+        <f>SUM(G3:G26)/30</f>
         <v>0.10804666666666665</v>
       </c>
     </row>

</xml_diff>